<commit_message>
modified:   TEST.xlsx 	modified:   Util.py 	modified:   Wrdwriter.py 	modified:   Xlreader.py 	modified:   __pycache__/UImaker.cpython-311.pyc 	modified:   __pycache__/Util.cpython-311.pyc 	modified:   __pycache__/Wrdwriter.cpython-311.pyc 	modified:   __pycache__/Xlreader.cpython-311.pyc 	modified:   finaldoc.docx 	modified:   main.py 	modified:   transferfile.txt
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuba\Protokolar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{660146AD-BDCB-46FD-9B55-6B674C9326DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57F7752-1A81-4CD2-979D-8864E0E4DFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
@@ -469,11 +469,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>